<commit_message>
Update file CTS6326_Project plan
</commit_message>
<xml_diff>
--- a/Document/CTS6326_Project plan.xlsx
+++ b/Document/CTS6326_Project plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TaiLieu\DATN\DA\Nhom28_MTTTN\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>TT</t>
   </si>
@@ -162,25 +162,10 @@
     <t>26/09/23</t>
   </si>
   <si>
-    <t>20/09/20</t>
-  </si>
-  <si>
-    <t>20/09/21</t>
-  </si>
-  <si>
-    <t>20/09/22</t>
-  </si>
-  <si>
-    <t>26/09/20</t>
-  </si>
-  <si>
-    <t>26/09/21</t>
-  </si>
-  <si>
-    <t>26/09/22</t>
-  </si>
-  <si>
-    <t>Cần tìm hiểu thêm</t>
+    <t>Nguyễn Phạm Nhật Minh</t>
+  </si>
+  <si>
+    <t>Bùi Phi Long</t>
   </si>
 </sst>
 </file>
@@ -275,7 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -294,6 +279,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +695,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -766,10 +753,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>43</v>
@@ -787,16 +774,16 @@
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -808,10 +795,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>43</v>
@@ -862,10 +849,18 @@
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -875,10 +870,18 @@
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -888,10 +891,18 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -901,10 +912,18 @@
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -914,10 +933,18 @@
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -927,10 +954,18 @@
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -940,10 +975,18 @@
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="C14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -953,10 +996,18 @@
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="C15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -966,10 +1017,18 @@
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="10">
+        <v>45026</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update file CTS6326_Project plan.xlsx
</commit_message>
<xml_diff>
--- a/Document/CTS6326_Project plan.xlsx
+++ b/Document/CTS6326_Project plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>TT</t>
   </si>
@@ -695,7 +695,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1051,10 +1051,18 @@
       <c r="B18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="C18" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D18" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1064,9 +1072,15 @@
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="C19" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D19" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
@@ -1077,9 +1091,15 @@
       <c r="B20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D20" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
@@ -1090,10 +1110,18 @@
       <c r="B21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="C21" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D21" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1103,10 +1131,18 @@
       <c r="B22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="C22" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D22" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1116,9 +1152,15 @@
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="C23" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D23" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
@@ -1129,9 +1171,15 @@
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="C24" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D24" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
@@ -1142,9 +1190,15 @@
       <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="C25" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D25" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
@@ -1168,9 +1222,15 @@
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="C27" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D27" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
@@ -1181,9 +1241,15 @@
       <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="C28" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D28" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
@@ -1194,9 +1260,15 @@
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="C29" s="10">
+        <v>45026</v>
+      </c>
+      <c r="D29" s="10">
+        <v>45240</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update docs, detailed layout design and test cases
</commit_message>
<xml_diff>
--- a/Document/CTS6326_Project plan.xlsx
+++ b/Document/CTS6326_Project plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
   <si>
     <t>TT</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Bùi Phi Long</t>
+  </si>
+  <si>
+    <t>18/10/23</t>
+  </si>
+  <si>
+    <t>25/10/23</t>
   </si>
 </sst>
 </file>
@@ -694,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1081,7 +1087,9 @@
       <c r="E19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1100,7 +1108,9 @@
       <c r="E20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1161,7 +1171,9 @@
       <c r="E23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1180,7 +1192,9 @@
       <c r="E24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1199,7 +1213,9 @@
       <c r="E25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1222,10 +1238,18 @@
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1235,10 +1259,18 @@
       <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="C28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1248,10 +1280,18 @@
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="C29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>